<commit_message>
Update tgl :) pantau 31.10.2015 jam 04.50
</commit_message>
<xml_diff>
--- a/pantauharian102015.xlsx
+++ b/pantauharian102015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="Buku_Kerja_Ini" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\putua\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\putua\Documents\GitHub\batur.10.2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1369,16 +1369,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2346920187064216</c:v>
+                  <c:v>1.2689944494157097</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.86021602112039275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37144376866075912</c:v>
+                  <c:v>0.37150612718660397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.019667451150154</c:v>
+                  <c:v>1.0204074343977068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,16 +1479,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.1173464331724167E-2</c:v>
+                  <c:v>3.0338208021291956E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.2169167803547066E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4351330926190275E-2</c:v>
+                  <c:v>2.4309345872869259E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8043229904492069E-2</c:v>
+                  <c:v>3.7974683544303799E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1504,12 +1504,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="232231840"/>
-        <c:axId val="232224392"/>
+        <c:axId val="376678016"/>
+        <c:axId val="376679584"/>
         <c:extLst/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="232231840"/>
+        <c:axId val="376678016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,7 +1552,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232224392"/>
+        <c:crossAx val="376679584"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1560,7 +1560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232224392"/>
+        <c:axId val="376679584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1613,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232231840"/>
+        <c:crossAx val="376678016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2540,8 +2540,8 @@
   </sheetPr>
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2564,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="str">
         <f>+"GRAFIK PROGRESS PENCAPAIAN RUPIAH DAN LEMBAR PER-TGL : "&amp;A21</f>
-        <v>GRAFIK PROGRESS PENCAPAIAN RUPIAH DAN LEMBAR PER-TGL : 30 - 21:20</v>
+        <v>GRAFIK PROGRESS PENCAPAIAN RUPIAH DAN LEMBAR PER-TGL : 31 - 04:50</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -2611,8 +2611,8 @@
       </c>
     </row>
     <row r="21" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
-        <v>253</v>
+      <c r="A21" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
@@ -2656,30 +2656,30 @@
       </c>
       <c r="C23" s="29">
         <f>VLOOKUP(A21,$A$30:$E$50,2,FALSE)</f>
-        <v>396647532</v>
+        <v>385925677</v>
       </c>
       <c r="D23" s="29">
         <f>+B23-C23</f>
-        <v>93090010</v>
+        <v>103811865</v>
       </c>
       <c r="E23" s="33">
         <f>+B23/C23*100%</f>
-        <v>1.2346920187064216</v>
+        <v>1.2689944494157097</v>
       </c>
       <c r="G23" s="28">
         <v>70637</v>
       </c>
       <c r="H23" s="29">
         <f>VLOOKUP($A$21,$A$30:$T$50,12,FALSE)</f>
-        <v>2202</v>
+        <v>2143</v>
       </c>
       <c r="I23" s="29">
         <f>+G23-H23</f>
-        <v>68435</v>
+        <v>68494</v>
       </c>
       <c r="J23" s="39">
         <f>+H23/G23</f>
-        <v>3.1173464331724167E-2</v>
+        <v>3.0338208021291956E-2</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2726,30 +2726,30 @@
       </c>
       <c r="C25" s="29">
         <f>VLOOKUP($A$21,$A$30:$E$50,4,FALSE)</f>
-        <v>50311793</v>
+        <v>50303348</v>
       </c>
       <c r="D25" s="29">
         <f t="shared" si="0"/>
-        <v>31623791</v>
+        <v>31615346</v>
       </c>
       <c r="E25" s="33">
         <f>+B25/C25*100%</f>
-        <v>0.37144376866075912</v>
+        <v>0.37150612718660397</v>
       </c>
       <c r="G25" s="28">
         <v>23818</v>
       </c>
       <c r="H25" s="29">
         <f>VLOOKUP($A$21,$A$30:$T$50,14,FALSE)</f>
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I25" s="29">
         <f t="shared" si="1"/>
-        <v>23238</v>
+        <v>23239</v>
       </c>
       <c r="J25" s="39">
         <f t="shared" si="2"/>
-        <v>2.4351330926190275E-2</v>
+        <v>2.4309345872869259E-2</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -2761,30 +2761,30 @@
       </c>
       <c r="C26" s="29">
         <f>VLOOKUP($A$21,$A$30:$E$50,5,FALSE)</f>
-        <v>192694517</v>
+        <v>192554778</v>
       </c>
       <c r="D26" s="29">
         <f t="shared" si="0"/>
-        <v>-3789810</v>
+        <v>-3929549</v>
       </c>
       <c r="E26" s="33">
         <f>+B26/C26*100%</f>
-        <v>1.019667451150154</v>
+        <v>1.0204074343977068</v>
       </c>
       <c r="G26" s="28">
         <v>43766</v>
       </c>
       <c r="H26" s="29">
         <f>VLOOKUP($A$21,$A$30:$T$50,15,FALSE)</f>
-        <v>1665</v>
+        <v>1662</v>
       </c>
       <c r="I26" s="29">
         <f t="shared" si="1"/>
-        <v>42101</v>
+        <v>42104</v>
       </c>
       <c r="J26" s="39">
         <f t="shared" si="2"/>
-        <v>3.8043229904492069E-2</v>
+        <v>3.7974683544303799E-2</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UPDATE TGL 31.10.2105 JAM 23:55
</commit_message>
<xml_diff>
--- a/pantauharian102015.xlsx
+++ b/pantauharian102015.xlsx
@@ -840,7 +840,7 @@
     <t>31 - 19:30</t>
   </si>
   <si>
-    <t>31 - 24:55</t>
+    <t>31 - 23:55</t>
   </si>
 </sst>
 </file>
@@ -1183,6 +1183,15 @@
     <xf numFmtId="10" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="41" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,15 +1200,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2610,8 +2610,8 @@
   </sheetPr>
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2632,47 +2632,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="str">
+      <c r="A1" s="63" t="str">
         <f>+"GRAFIK PROGRESS PENCAPAIAN RUPIAH DAN LEMBAR PER-TGL : "&amp;A21</f>
-        <v>GRAFIK PROGRESS PENCAPAIAN RUPIAH DAN LEMBAR PER-TGL : 31 - 24:55</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
+        <v>GRAFIK PROGRESS PENCAPAIAN RUPIAH DAN LEMBAR PER-TGL : 31 - 23:55</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
       <c r="K1" s="35"/>
       <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
       <c r="K2" s="35"/>
       <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
     </row>
     <row r="19" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -2906,39 +2906,39 @@
       <c r="J28" s="53"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+      <c r="A29" s="64" t="s">
         <v>241</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="62" t="s">
         <v>243</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="59" t="s">
+      <c r="G29" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="59" t="s">
+      <c r="L29" s="62" t="s">
         <v>244</v>
       </c>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
       <c r="P29" s="24"/>
-      <c r="Q29" s="59" t="s">
+      <c r="Q29" s="62" t="s">
         <v>246</v>
       </c>
-      <c r="R29" s="59"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="59"/>
+      <c r="R29" s="62"/>
+      <c r="S29" s="62"/>
+      <c r="T29" s="62"/>
     </row>
     <row r="30" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="23" t="s">
         <v>20</v>
       </c>
@@ -4777,7 +4777,7 @@
       <pane xSplit="5" ySplit="5" topLeftCell="Q6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AA5" sqref="AA5:AA188"/>
+      <selection pane="bottomRight" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4898,7 +4898,7 @@
       <c r="Z5" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="AA5" s="62" t="s">
+      <c r="AA5" s="59" t="s">
         <v>258</v>
       </c>
     </row>
@@ -4981,7 +4981,7 @@
       <c r="Z6" s="3">
         <v>185489</v>
       </c>
-      <c r="AA6" s="63">
+      <c r="AA6" s="60">
         <v>185489</v>
       </c>
     </row>
@@ -5064,7 +5064,7 @@
       <c r="Z7" s="3">
         <v>291748</v>
       </c>
-      <c r="AA7" s="63">
+      <c r="AA7" s="60">
         <v>291748</v>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       <c r="Z8" s="3">
         <v>7359040</v>
       </c>
-      <c r="AA8" s="63">
+      <c r="AA8" s="60">
         <v>7359040</v>
       </c>
     </row>
@@ -5230,7 +5230,7 @@
       <c r="Z9" s="3">
         <v>498817</v>
       </c>
-      <c r="AA9" s="63">
+      <c r="AA9" s="60">
         <v>498817</v>
       </c>
     </row>
@@ -5313,7 +5313,7 @@
       <c r="Z10" s="3">
         <v>948627</v>
       </c>
-      <c r="AA10" s="63">
+      <c r="AA10" s="60">
         <v>948627</v>
       </c>
     </row>
@@ -5396,7 +5396,7 @@
       <c r="Z11" s="3">
         <v>1230350</v>
       </c>
-      <c r="AA11" s="63">
+      <c r="AA11" s="60">
         <v>1230350</v>
       </c>
     </row>
@@ -5479,7 +5479,7 @@
       <c r="Z12" s="3">
         <v>1531448</v>
       </c>
-      <c r="AA12" s="63">
+      <c r="AA12" s="60">
         <v>1531448</v>
       </c>
     </row>
@@ -5534,7 +5534,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="64"/>
+      <c r="AA13" s="61"/>
     </row>
     <row r="14" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
@@ -5615,7 +5615,7 @@
       <c r="Z14" s="3">
         <v>6754469</v>
       </c>
-      <c r="AA14" s="63">
+      <c r="AA14" s="60">
         <v>6754469</v>
       </c>
     </row>
@@ -5698,7 +5698,7 @@
       <c r="Z15" s="3">
         <v>359719</v>
       </c>
-      <c r="AA15" s="63">
+      <c r="AA15" s="60">
         <v>359719</v>
       </c>
     </row>
@@ -5781,7 +5781,7 @@
       <c r="Z16" s="3">
         <v>2936120</v>
       </c>
-      <c r="AA16" s="63">
+      <c r="AA16" s="60">
         <v>2936120</v>
       </c>
     </row>
@@ -5864,7 +5864,7 @@
       <c r="Z17" s="3">
         <v>1545638</v>
       </c>
-      <c r="AA17" s="63">
+      <c r="AA17" s="60">
         <v>1545638</v>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       <c r="Z18" s="3">
         <v>1757290</v>
       </c>
-      <c r="AA18" s="63">
+      <c r="AA18" s="60">
         <v>1588525</v>
       </c>
     </row>
@@ -6030,7 +6030,7 @@
       <c r="Z19" s="3">
         <v>16088384</v>
       </c>
-      <c r="AA19" s="63">
+      <c r="AA19" s="60">
         <v>16088384</v>
       </c>
     </row>
@@ -6113,7 +6113,7 @@
       <c r="Z20" s="3">
         <v>4899128</v>
       </c>
-      <c r="AA20" s="63">
+      <c r="AA20" s="60">
         <v>4029958</v>
       </c>
     </row>
@@ -6196,7 +6196,7 @@
       <c r="Z21" s="3">
         <v>625019</v>
       </c>
-      <c r="AA21" s="63">
+      <c r="AA21" s="60">
         <v>625019</v>
       </c>
     </row>
@@ -6279,7 +6279,7 @@
       <c r="Z22" s="3">
         <v>2463136</v>
       </c>
-      <c r="AA22" s="63">
+      <c r="AA22" s="60">
         <v>2463136</v>
       </c>
     </row>
@@ -6362,7 +6362,7 @@
       <c r="Z23" s="3">
         <v>3515142</v>
       </c>
-      <c r="AA23" s="63">
+      <c r="AA23" s="60">
         <v>3515142</v>
       </c>
     </row>
@@ -6445,7 +6445,7 @@
       <c r="Z24" s="3">
         <v>452860</v>
       </c>
-      <c r="AA24" s="63">
+      <c r="AA24" s="60">
         <v>452860</v>
       </c>
     </row>
@@ -6528,7 +6528,7 @@
       <c r="Z25" s="3">
         <v>6958006</v>
       </c>
-      <c r="AA25" s="63">
+      <c r="AA25" s="60">
         <v>5282246</v>
       </c>
     </row>
@@ -6611,7 +6611,7 @@
       <c r="Z26" s="3">
         <v>7440102</v>
       </c>
-      <c r="AA26" s="63">
+      <c r="AA26" s="60">
         <v>7440102</v>
       </c>
     </row>
@@ -6694,7 +6694,7 @@
       <c r="Z27" s="3">
         <v>6376818</v>
       </c>
-      <c r="AA27" s="63">
+      <c r="AA27" s="60">
         <v>6376818</v>
       </c>
     </row>
@@ -6777,7 +6777,7 @@
       <c r="Z28" s="3">
         <v>2963082</v>
       </c>
-      <c r="AA28" s="63">
+      <c r="AA28" s="60">
         <v>2963082</v>
       </c>
     </row>
@@ -6858,7 +6858,7 @@
         <v>574440</v>
       </c>
       <c r="Z29" s="5"/>
-      <c r="AA29" s="64"/>
+      <c r="AA29" s="61"/>
     </row>
     <row r="30" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
@@ -6939,7 +6939,7 @@
       <c r="Z30" s="3">
         <v>11288597</v>
       </c>
-      <c r="AA30" s="63">
+      <c r="AA30" s="60">
         <v>11288597</v>
       </c>
     </row>
@@ -7022,7 +7022,7 @@
       <c r="Z31" s="3">
         <v>6943008</v>
       </c>
-      <c r="AA31" s="63">
+      <c r="AA31" s="60">
         <v>6822319</v>
       </c>
     </row>
@@ -7105,7 +7105,7 @@
       <c r="Z32" s="3">
         <v>3751851</v>
       </c>
-      <c r="AA32" s="63">
+      <c r="AA32" s="60">
         <v>3751851</v>
       </c>
     </row>
@@ -7188,7 +7188,7 @@
       <c r="Z33" s="3">
         <v>62972</v>
       </c>
-      <c r="AA33" s="63">
+      <c r="AA33" s="60">
         <v>62972</v>
       </c>
     </row>
@@ -7271,7 +7271,7 @@
       <c r="Z34" s="3">
         <v>5464692</v>
       </c>
-      <c r="AA34" s="63">
+      <c r="AA34" s="60">
         <v>5384681</v>
       </c>
     </row>
@@ -7354,7 +7354,7 @@
       <c r="Z35" s="3">
         <v>606904</v>
       </c>
-      <c r="AA35" s="63">
+      <c r="AA35" s="60">
         <v>606904</v>
       </c>
     </row>
@@ -7437,7 +7437,7 @@
       <c r="Z36" s="3">
         <v>22800</v>
       </c>
-      <c r="AA36" s="63">
+      <c r="AA36" s="60">
         <v>22800</v>
       </c>
     </row>
@@ -7520,7 +7520,7 @@
       <c r="Z37" s="3">
         <v>2259818</v>
       </c>
-      <c r="AA37" s="63">
+      <c r="AA37" s="60">
         <v>2203424</v>
       </c>
     </row>
@@ -7603,7 +7603,7 @@
       <c r="Z38" s="3">
         <v>216132</v>
       </c>
-      <c r="AA38" s="63">
+      <c r="AA38" s="60">
         <v>216132</v>
       </c>
     </row>
@@ -7686,7 +7686,7 @@
       <c r="Z39" s="3">
         <v>9091867</v>
       </c>
-      <c r="AA39" s="63">
+      <c r="AA39" s="60">
         <v>9022638</v>
       </c>
     </row>
@@ -7769,7 +7769,7 @@
       <c r="Z40" s="3">
         <v>1489173</v>
       </c>
-      <c r="AA40" s="63">
+      <c r="AA40" s="60">
         <v>1489173</v>
       </c>
     </row>
@@ -7852,7 +7852,7 @@
       <c r="Z41" s="3">
         <v>6351434</v>
       </c>
-      <c r="AA41" s="63">
+      <c r="AA41" s="60">
         <v>6351434</v>
       </c>
     </row>
@@ -7935,7 +7935,7 @@
       <c r="Z42" s="3">
         <v>4634847</v>
       </c>
-      <c r="AA42" s="63">
+      <c r="AA42" s="60">
         <v>4634847</v>
       </c>
     </row>
@@ -8018,7 +8018,7 @@
       <c r="Z43" s="3">
         <v>6421764</v>
       </c>
-      <c r="AA43" s="63">
+      <c r="AA43" s="60">
         <v>6370815</v>
       </c>
     </row>
@@ -8101,7 +8101,7 @@
       <c r="Z44" s="3">
         <v>3252823</v>
       </c>
-      <c r="AA44" s="63">
+      <c r="AA44" s="60">
         <v>3252823</v>
       </c>
     </row>
@@ -8184,7 +8184,7 @@
       <c r="Z45" s="3">
         <v>6868126</v>
       </c>
-      <c r="AA45" s="63">
+      <c r="AA45" s="60">
         <v>6868126</v>
       </c>
     </row>
@@ -8267,7 +8267,7 @@
       <c r="Z46" s="3">
         <v>1168071</v>
       </c>
-      <c r="AA46" s="63">
+      <c r="AA46" s="60">
         <v>1168071</v>
       </c>
     </row>
@@ -8350,7 +8350,7 @@
       <c r="Z47" s="3">
         <v>12402061</v>
       </c>
-      <c r="AA47" s="63">
+      <c r="AA47" s="60">
         <v>11720506</v>
       </c>
     </row>
@@ -8433,7 +8433,7 @@
       <c r="Z48" s="3">
         <v>4397858</v>
       </c>
-      <c r="AA48" s="63">
+      <c r="AA48" s="60">
         <v>4397858</v>
       </c>
     </row>
@@ -8516,7 +8516,7 @@
       <c r="Z49" s="3">
         <v>2956006</v>
       </c>
-      <c r="AA49" s="63">
+      <c r="AA49" s="60">
         <v>2956006</v>
       </c>
     </row>
@@ -8599,7 +8599,7 @@
       <c r="Z50" s="3">
         <v>211975</v>
       </c>
-      <c r="AA50" s="63">
+      <c r="AA50" s="60">
         <v>211975</v>
       </c>
     </row>
@@ -8682,7 +8682,7 @@
       <c r="Z51" s="3">
         <v>9417534</v>
       </c>
-      <c r="AA51" s="63">
+      <c r="AA51" s="60">
         <v>9417534</v>
       </c>
     </row>
@@ -8765,7 +8765,7 @@
       <c r="Z52" s="3">
         <v>2505030</v>
       </c>
-      <c r="AA52" s="63">
+      <c r="AA52" s="60">
         <v>2505030</v>
       </c>
     </row>
@@ -8848,7 +8848,7 @@
       <c r="Z53" s="3">
         <v>5321240</v>
       </c>
-      <c r="AA53" s="63">
+      <c r="AA53" s="60">
         <v>5321240</v>
       </c>
     </row>
@@ -8931,7 +8931,7 @@
       <c r="Z54" s="3">
         <v>186526</v>
       </c>
-      <c r="AA54" s="63">
+      <c r="AA54" s="60">
         <v>186526</v>
       </c>
     </row>
@@ -9014,7 +9014,7 @@
       <c r="Z55" s="3">
         <v>2396374</v>
       </c>
-      <c r="AA55" s="63">
+      <c r="AA55" s="60">
         <v>2396374</v>
       </c>
     </row>
@@ -9073,7 +9073,7 @@
       <c r="X56" s="5"/>
       <c r="Y56" s="10"/>
       <c r="Z56" s="5"/>
-      <c r="AA56" s="64"/>
+      <c r="AA56" s="61"/>
     </row>
     <row r="57" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
@@ -9154,7 +9154,7 @@
       <c r="Z57" s="3">
         <v>9326297</v>
       </c>
-      <c r="AA57" s="63">
+      <c r="AA57" s="60">
         <v>9326297</v>
       </c>
     </row>
@@ -9237,7 +9237,7 @@
       <c r="Z58" s="3">
         <v>859909</v>
       </c>
-      <c r="AA58" s="63">
+      <c r="AA58" s="60">
         <v>859909</v>
       </c>
     </row>
@@ -9320,7 +9320,7 @@
       <c r="Z59" s="3">
         <v>2236991</v>
       </c>
-      <c r="AA59" s="63">
+      <c r="AA59" s="60">
         <v>2236991</v>
       </c>
     </row>
@@ -9403,7 +9403,7 @@
       <c r="Z60" s="3">
         <v>384530</v>
       </c>
-      <c r="AA60" s="63">
+      <c r="AA60" s="60">
         <v>384530</v>
       </c>
     </row>
@@ -9486,7 +9486,7 @@
       <c r="Z61" s="3">
         <v>5621611</v>
       </c>
-      <c r="AA61" s="63">
+      <c r="AA61" s="60">
         <v>5426249</v>
       </c>
     </row>
@@ -9569,7 +9569,7 @@
       <c r="Z62" s="3">
         <v>993584</v>
       </c>
-      <c r="AA62" s="63">
+      <c r="AA62" s="60">
         <v>993584</v>
       </c>
     </row>
@@ -9652,7 +9652,7 @@
       <c r="Z63" s="3">
         <v>8741793</v>
       </c>
-      <c r="AA63" s="63">
+      <c r="AA63" s="60">
         <v>8741793</v>
       </c>
     </row>
@@ -9735,7 +9735,7 @@
       <c r="Z64" s="3">
         <v>1071555</v>
       </c>
-      <c r="AA64" s="63">
+      <c r="AA64" s="60">
         <v>1071555</v>
       </c>
     </row>
@@ -9814,7 +9814,7 @@
       </c>
       <c r="Y65" s="10"/>
       <c r="Z65" s="5"/>
-      <c r="AA65" s="64"/>
+      <c r="AA65" s="61"/>
     </row>
     <row r="66" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
@@ -9895,7 +9895,7 @@
       <c r="Z66" s="3">
         <v>169668</v>
       </c>
-      <c r="AA66" s="63">
+      <c r="AA66" s="60">
         <v>169668</v>
       </c>
     </row>
@@ -9978,7 +9978,7 @@
       <c r="Z67" s="3">
         <v>8460297</v>
       </c>
-      <c r="AA67" s="63">
+      <c r="AA67" s="60">
         <v>8460297</v>
       </c>
     </row>
@@ -10061,7 +10061,7 @@
       <c r="Z68" s="3">
         <v>489417</v>
       </c>
-      <c r="AA68" s="63">
+      <c r="AA68" s="60">
         <v>489417</v>
       </c>
     </row>
@@ -10144,7 +10144,7 @@
       <c r="Z69" s="3">
         <v>10487243</v>
       </c>
-      <c r="AA69" s="63">
+      <c r="AA69" s="60">
         <v>10487243</v>
       </c>
     </row>
@@ -10227,7 +10227,7 @@
       <c r="Z70" s="3">
         <v>4053220</v>
       </c>
-      <c r="AA70" s="63">
+      <c r="AA70" s="60">
         <v>4053220</v>
       </c>
     </row>
@@ -10310,7 +10310,7 @@
       <c r="Z71" s="3">
         <v>2846060</v>
       </c>
-      <c r="AA71" s="63">
+      <c r="AA71" s="60">
         <v>2846060</v>
       </c>
     </row>
@@ -10393,7 +10393,7 @@
       <c r="Z72" s="3">
         <v>48600</v>
       </c>
-      <c r="AA72" s="63">
+      <c r="AA72" s="60">
         <v>48600</v>
       </c>
     </row>
@@ -10476,7 +10476,7 @@
       <c r="Z73" s="3">
         <v>8416857</v>
       </c>
-      <c r="AA73" s="63">
+      <c r="AA73" s="60">
         <v>8214059</v>
       </c>
     </row>
@@ -10559,7 +10559,7 @@
       <c r="Z74" s="3">
         <v>4097648</v>
       </c>
-      <c r="AA74" s="63">
+      <c r="AA74" s="60">
         <v>4097648</v>
       </c>
     </row>
@@ -10642,7 +10642,7 @@
       <c r="Z75" s="3">
         <v>4860203</v>
       </c>
-      <c r="AA75" s="63">
+      <c r="AA75" s="60">
         <v>4860203</v>
       </c>
     </row>
@@ -10725,7 +10725,7 @@
       <c r="Z76" s="3">
         <v>1881229</v>
       </c>
-      <c r="AA76" s="63">
+      <c r="AA76" s="60">
         <v>1881229</v>
       </c>
     </row>
@@ -10808,7 +10808,7 @@
       <c r="Z77" s="3">
         <v>4232216</v>
       </c>
-      <c r="AA77" s="63">
+      <c r="AA77" s="60">
         <v>4232216</v>
       </c>
     </row>
@@ -10891,7 +10891,7 @@
       <c r="Z78" s="3">
         <v>1993428</v>
       </c>
-      <c r="AA78" s="63">
+      <c r="AA78" s="60">
         <v>1993428</v>
       </c>
     </row>
@@ -10974,7 +10974,7 @@
       <c r="Z79" s="3">
         <v>5106132</v>
       </c>
-      <c r="AA79" s="63">
+      <c r="AA79" s="60">
         <v>4710922</v>
       </c>
     </row>
@@ -11057,7 +11057,7 @@
       <c r="Z80" s="3">
         <v>404647</v>
       </c>
-      <c r="AA80" s="63">
+      <c r="AA80" s="60">
         <v>404647</v>
       </c>
     </row>
@@ -11140,7 +11140,7 @@
       <c r="Z81" s="3">
         <v>7523451</v>
       </c>
-      <c r="AA81" s="63">
+      <c r="AA81" s="60">
         <v>7523451</v>
       </c>
     </row>
@@ -11223,7 +11223,7 @@
       <c r="Z82" s="3">
         <v>1468301</v>
       </c>
-      <c r="AA82" s="63">
+      <c r="AA82" s="60">
         <v>1468301</v>
       </c>
     </row>
@@ -11306,7 +11306,7 @@
       <c r="Z83" s="3">
         <v>13271874</v>
       </c>
-      <c r="AA83" s="63">
+      <c r="AA83" s="60">
         <v>13271874</v>
       </c>
     </row>
@@ -11389,7 +11389,7 @@
       <c r="Z84" s="3">
         <v>3196923</v>
       </c>
-      <c r="AA84" s="63">
+      <c r="AA84" s="60">
         <v>3196923</v>
       </c>
     </row>
@@ -11472,7 +11472,7 @@
       <c r="Z85" s="3">
         <v>3293591</v>
       </c>
-      <c r="AA85" s="63">
+      <c r="AA85" s="60">
         <v>3293591</v>
       </c>
     </row>
@@ -11555,7 +11555,7 @@
       <c r="Z86" s="3">
         <v>1329942</v>
       </c>
-      <c r="AA86" s="63">
+      <c r="AA86" s="60">
         <v>1329942</v>
       </c>
     </row>
@@ -11638,7 +11638,7 @@
       <c r="Z87" s="3">
         <v>2648112</v>
       </c>
-      <c r="AA87" s="63">
+      <c r="AA87" s="60">
         <v>2648112</v>
       </c>
     </row>
@@ -11721,7 +11721,7 @@
       <c r="Z88" s="3">
         <v>5981881</v>
       </c>
-      <c r="AA88" s="63">
+      <c r="AA88" s="60">
         <v>5981881</v>
       </c>
     </row>
@@ -11802,7 +11802,7 @@
         <v>363314</v>
       </c>
       <c r="Z89" s="5"/>
-      <c r="AA89" s="64"/>
+      <c r="AA89" s="61"/>
     </row>
     <row r="90" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90" s="14">
@@ -11883,7 +11883,7 @@
       <c r="Z90" s="3">
         <v>1371396</v>
       </c>
-      <c r="AA90" s="63">
+      <c r="AA90" s="60">
         <v>1371396</v>
       </c>
     </row>
@@ -11962,7 +11962,7 @@
       </c>
       <c r="Y91" s="10"/>
       <c r="Z91" s="5"/>
-      <c r="AA91" s="64"/>
+      <c r="AA91" s="61"/>
     </row>
     <row r="92" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92" s="14">
@@ -12043,7 +12043,7 @@
       <c r="Z92" s="3">
         <v>350790</v>
       </c>
-      <c r="AA92" s="63">
+      <c r="AA92" s="60">
         <v>350790</v>
       </c>
     </row>
@@ -12126,7 +12126,7 @@
       <c r="Z93" s="3">
         <v>1325974</v>
       </c>
-      <c r="AA93" s="63">
+      <c r="AA93" s="60">
         <v>1325974</v>
       </c>
     </row>
@@ -12209,7 +12209,7 @@
       <c r="Z94" s="3">
         <v>1273009</v>
       </c>
-      <c r="AA94" s="63">
+      <c r="AA94" s="60">
         <v>1251859</v>
       </c>
     </row>
@@ -12276,7 +12276,7 @@
       <c r="X95" s="5"/>
       <c r="Y95" s="10"/>
       <c r="Z95" s="5"/>
-      <c r="AA95" s="64"/>
+      <c r="AA95" s="61"/>
     </row>
     <row r="96" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
@@ -12357,7 +12357,7 @@
       <c r="Z96" s="3">
         <v>1148620</v>
       </c>
-      <c r="AA96" s="63">
+      <c r="AA96" s="60">
         <v>1148620</v>
       </c>
     </row>
@@ -12440,7 +12440,7 @@
       <c r="Z97" s="3">
         <v>177598</v>
       </c>
-      <c r="AA97" s="63">
+      <c r="AA97" s="60">
         <v>177598</v>
       </c>
     </row>
@@ -12523,7 +12523,7 @@
       <c r="Z98" s="3">
         <v>70248</v>
       </c>
-      <c r="AA98" s="63">
+      <c r="AA98" s="60">
         <v>70248</v>
       </c>
     </row>
@@ -12606,7 +12606,7 @@
       <c r="Z99" s="3">
         <v>835051</v>
       </c>
-      <c r="AA99" s="63">
+      <c r="AA99" s="60">
         <v>835051</v>
       </c>
     </row>
@@ -12669,7 +12669,7 @@
       <c r="X100" s="5"/>
       <c r="Y100" s="10"/>
       <c r="Z100" s="5"/>
-      <c r="AA100" s="64"/>
+      <c r="AA100" s="61"/>
     </row>
     <row r="101" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="14">
@@ -12750,7 +12750,7 @@
       <c r="Z101" s="3">
         <v>2026141</v>
       </c>
-      <c r="AA101" s="63">
+      <c r="AA101" s="60">
         <v>1920772</v>
       </c>
     </row>
@@ -12793,7 +12793,7 @@
       <c r="X102" s="5"/>
       <c r="Y102" s="10"/>
       <c r="Z102" s="5"/>
-      <c r="AA102" s="64"/>
+      <c r="AA102" s="61"/>
     </row>
     <row r="103" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="14">
@@ -12874,7 +12874,7 @@
       <c r="Z103" s="3">
         <v>1970795</v>
       </c>
-      <c r="AA103" s="63">
+      <c r="AA103" s="60">
         <v>1970795</v>
       </c>
     </row>
@@ -12957,7 +12957,7 @@
       <c r="Z104" s="3">
         <v>1168162</v>
       </c>
-      <c r="AA104" s="63">
+      <c r="AA104" s="60">
         <v>1168162</v>
       </c>
     </row>
@@ -13040,7 +13040,7 @@
       <c r="Z105" s="3">
         <v>728112</v>
       </c>
-      <c r="AA105" s="63">
+      <c r="AA105" s="60">
         <v>728112</v>
       </c>
     </row>
@@ -13107,7 +13107,7 @@
       <c r="X106" s="5"/>
       <c r="Y106" s="10"/>
       <c r="Z106" s="5"/>
-      <c r="AA106" s="64"/>
+      <c r="AA106" s="61"/>
     </row>
     <row r="107" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A107" s="14">
@@ -13188,7 +13188,7 @@
       <c r="Z107" s="3">
         <v>1104560</v>
       </c>
-      <c r="AA107" s="63">
+      <c r="AA107" s="60">
         <v>1104560</v>
       </c>
     </row>
@@ -13261,7 +13261,7 @@
       <c r="X108" s="5"/>
       <c r="Y108" s="10"/>
       <c r="Z108" s="5"/>
-      <c r="AA108" s="64"/>
+      <c r="AA108" s="61"/>
     </row>
     <row r="109" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A109" s="14">
@@ -13342,7 +13342,7 @@
       <c r="Z109" s="3">
         <v>222121</v>
       </c>
-      <c r="AA109" s="63">
+      <c r="AA109" s="60">
         <v>187410</v>
       </c>
     </row>
@@ -13425,7 +13425,7 @@
       <c r="Z110" s="3">
         <v>19890</v>
       </c>
-      <c r="AA110" s="63">
+      <c r="AA110" s="60">
         <v>19890</v>
       </c>
     </row>
@@ -13508,7 +13508,7 @@
       <c r="Z111" s="3">
         <v>2156780</v>
       </c>
-      <c r="AA111" s="63">
+      <c r="AA111" s="60">
         <v>2091470</v>
       </c>
     </row>
@@ -13591,7 +13591,7 @@
       <c r="Z112" s="3">
         <v>106149</v>
       </c>
-      <c r="AA112" s="63">
+      <c r="AA112" s="60">
         <v>106149</v>
       </c>
     </row>
@@ -13674,7 +13674,7 @@
       <c r="Z113" s="3">
         <v>1779711</v>
       </c>
-      <c r="AA113" s="63">
+      <c r="AA113" s="60">
         <v>1779711</v>
       </c>
     </row>
@@ -13753,7 +13753,7 @@
       </c>
       <c r="Y114" s="10"/>
       <c r="Z114" s="5"/>
-      <c r="AA114" s="64"/>
+      <c r="AA114" s="61"/>
     </row>
     <row r="115" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A115" s="14">
@@ -13832,7 +13832,7 @@
         <v>1234257</v>
       </c>
       <c r="Z115" s="5"/>
-      <c r="AA115" s="64"/>
+      <c r="AA115" s="61"/>
     </row>
     <row r="116" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A116" s="14">
@@ -13911,7 +13911,7 @@
         <v>815159</v>
       </c>
       <c r="Z116" s="5"/>
-      <c r="AA116" s="64"/>
+      <c r="AA116" s="61"/>
     </row>
     <row r="117" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A117" s="14">
@@ -13990,7 +13990,7 @@
         <v>1015973</v>
       </c>
       <c r="Z117" s="5"/>
-      <c r="AA117" s="64"/>
+      <c r="AA117" s="61"/>
     </row>
     <row r="118" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" s="14">
@@ -14069,7 +14069,7 @@
         <v>2521250</v>
       </c>
       <c r="Z118" s="5"/>
-      <c r="AA118" s="64"/>
+      <c r="AA118" s="61"/>
     </row>
     <row r="119" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A119" s="14">
@@ -14130,7 +14130,7 @@
       <c r="X119" s="5"/>
       <c r="Y119" s="10"/>
       <c r="Z119" s="5"/>
-      <c r="AA119" s="64"/>
+      <c r="AA119" s="61"/>
     </row>
     <row r="120" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A120" s="14">
@@ -14209,7 +14209,7 @@
         <v>1483269</v>
       </c>
       <c r="Z120" s="5"/>
-      <c r="AA120" s="64"/>
+      <c r="AA120" s="61"/>
     </row>
     <row r="121" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A121" s="14">
@@ -14288,7 +14288,7 @@
         <v>834362</v>
       </c>
       <c r="Z121" s="5"/>
-      <c r="AA121" s="64"/>
+      <c r="AA121" s="61"/>
     </row>
     <row r="122" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A122" s="14">
@@ -14367,7 +14367,7 @@
         <v>776403</v>
       </c>
       <c r="Z122" s="5"/>
-      <c r="AA122" s="64"/>
+      <c r="AA122" s="61"/>
     </row>
     <row r="123" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A123" s="14">
@@ -14446,7 +14446,7 @@
         <v>11550603</v>
       </c>
       <c r="Z123" s="5"/>
-      <c r="AA123" s="64"/>
+      <c r="AA123" s="61"/>
     </row>
     <row r="124" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A124" s="14">
@@ -14523,7 +14523,7 @@
       </c>
       <c r="Y124" s="10"/>
       <c r="Z124" s="5"/>
-      <c r="AA124" s="64"/>
+      <c r="AA124" s="61"/>
     </row>
     <row r="125" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" s="14">
@@ -14602,7 +14602,7 @@
         <v>1623029</v>
       </c>
       <c r="Z125" s="5"/>
-      <c r="AA125" s="64"/>
+      <c r="AA125" s="61"/>
     </row>
     <row r="126" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A126" s="14">
@@ -14681,7 +14681,7 @@
         <v>1198791</v>
       </c>
       <c r="Z126" s="5"/>
-      <c r="AA126" s="64"/>
+      <c r="AA126" s="61"/>
     </row>
     <row r="127" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" s="14">
@@ -14760,7 +14760,7 @@
         <v>1031925</v>
       </c>
       <c r="Z127" s="5"/>
-      <c r="AA127" s="64"/>
+      <c r="AA127" s="61"/>
     </row>
     <row r="128" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A128" s="14">
@@ -14839,7 +14839,7 @@
         <v>1238402</v>
       </c>
       <c r="Z128" s="5"/>
-      <c r="AA128" s="64"/>
+      <c r="AA128" s="61"/>
     </row>
     <row r="129" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" s="14">
@@ -14918,7 +14918,7 @@
         <v>4517622</v>
       </c>
       <c r="Z129" s="5"/>
-      <c r="AA129" s="64"/>
+      <c r="AA129" s="61"/>
     </row>
     <row r="130" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" s="14">
@@ -14997,7 +14997,7 @@
         <v>959595</v>
       </c>
       <c r="Z130" s="5"/>
-      <c r="AA130" s="64"/>
+      <c r="AA130" s="61"/>
     </row>
     <row r="131" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A131" s="14">
@@ -15078,7 +15078,7 @@
       <c r="Z131" s="3">
         <v>2139767</v>
       </c>
-      <c r="AA131" s="63">
+      <c r="AA131" s="60">
         <v>2139767</v>
       </c>
     </row>
@@ -15161,7 +15161,7 @@
       <c r="Z132" s="3">
         <v>155267</v>
       </c>
-      <c r="AA132" s="63">
+      <c r="AA132" s="60">
         <v>155267</v>
       </c>
     </row>
@@ -15242,7 +15242,7 @@
         <v>130206</v>
       </c>
       <c r="Z133" s="5"/>
-      <c r="AA133" s="64"/>
+      <c r="AA133" s="61"/>
     </row>
     <row r="134" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A134" s="14">
@@ -15283,7 +15283,7 @@
       <c r="X134" s="5"/>
       <c r="Y134" s="10"/>
       <c r="Z134" s="5"/>
-      <c r="AA134" s="64"/>
+      <c r="AA134" s="61"/>
     </row>
     <row r="135" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" s="14">
@@ -15364,7 +15364,7 @@
       <c r="Z135" s="3">
         <v>3394233</v>
       </c>
-      <c r="AA135" s="63">
+      <c r="AA135" s="60">
         <v>3394233</v>
       </c>
     </row>
@@ -15447,7 +15447,7 @@
       <c r="Z136" s="3">
         <v>2450315</v>
       </c>
-      <c r="AA136" s="63">
+      <c r="AA136" s="60">
         <v>2450315</v>
       </c>
     </row>
@@ -15530,7 +15530,7 @@
       <c r="Z137" s="3">
         <v>3189189</v>
       </c>
-      <c r="AA137" s="63">
+      <c r="AA137" s="60">
         <v>3189189</v>
       </c>
     </row>
@@ -15613,7 +15613,7 @@
       <c r="Z138" s="3">
         <v>739147</v>
       </c>
-      <c r="AA138" s="63">
+      <c r="AA138" s="60">
         <v>739147</v>
       </c>
     </row>
@@ -15696,7 +15696,7 @@
       <c r="Z139" s="3">
         <v>900886</v>
       </c>
-      <c r="AA139" s="63">
+      <c r="AA139" s="60">
         <v>900886</v>
       </c>
     </row>
@@ -15779,7 +15779,7 @@
       <c r="Z140" s="3">
         <v>19692</v>
       </c>
-      <c r="AA140" s="63">
+      <c r="AA140" s="60">
         <v>19692</v>
       </c>
     </row>
@@ -15862,7 +15862,7 @@
       <c r="Z141" s="3">
         <v>1201284</v>
       </c>
-      <c r="AA141" s="63">
+      <c r="AA141" s="60">
         <v>1201284</v>
       </c>
     </row>
@@ -15945,7 +15945,7 @@
       <c r="Z142" s="3">
         <v>390451</v>
       </c>
-      <c r="AA142" s="63">
+      <c r="AA142" s="60">
         <v>390451</v>
       </c>
     </row>
@@ -16028,7 +16028,7 @@
       <c r="Z143" s="3">
         <v>4712427</v>
       </c>
-      <c r="AA143" s="63">
+      <c r="AA143" s="60">
         <v>4712427</v>
       </c>
     </row>
@@ -16111,7 +16111,7 @@
       <c r="Z144" s="3">
         <v>622347</v>
       </c>
-      <c r="AA144" s="63">
+      <c r="AA144" s="60">
         <v>622347</v>
       </c>
     </row>
@@ -16194,7 +16194,7 @@
       <c r="Z145" s="3">
         <v>4173562</v>
       </c>
-      <c r="AA145" s="63">
+      <c r="AA145" s="60">
         <v>4173562</v>
       </c>
     </row>
@@ -16277,7 +16277,7 @@
       <c r="Z146" s="3">
         <v>386205</v>
       </c>
-      <c r="AA146" s="63">
+      <c r="AA146" s="60">
         <v>386205</v>
       </c>
     </row>
@@ -16360,7 +16360,7 @@
       <c r="Z147" s="3">
         <v>3936629</v>
       </c>
-      <c r="AA147" s="63">
+      <c r="AA147" s="60">
         <v>2677188</v>
       </c>
     </row>
@@ -16443,7 +16443,7 @@
       <c r="Z148" s="3">
         <v>127212</v>
       </c>
-      <c r="AA148" s="63">
+      <c r="AA148" s="60">
         <v>127212</v>
       </c>
     </row>
@@ -16526,7 +16526,7 @@
       <c r="Z149" s="3">
         <v>11819484</v>
       </c>
-      <c r="AA149" s="63">
+      <c r="AA149" s="60">
         <v>11819484</v>
       </c>
     </row>
@@ -16609,7 +16609,7 @@
       <c r="Z150" s="3">
         <v>16860620</v>
       </c>
-      <c r="AA150" s="63">
+      <c r="AA150" s="60">
         <v>16860620</v>
       </c>
     </row>
@@ -16686,7 +16686,7 @@
       <c r="X151" s="5"/>
       <c r="Y151" s="10"/>
       <c r="Z151" s="5"/>
-      <c r="AA151" s="64"/>
+      <c r="AA151" s="61"/>
     </row>
     <row r="152" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" s="14">
@@ -16767,7 +16767,7 @@
       <c r="Z152" s="3">
         <v>5234659</v>
       </c>
-      <c r="AA152" s="63">
+      <c r="AA152" s="60">
         <v>5234659</v>
       </c>
     </row>
@@ -16850,7 +16850,7 @@
       <c r="Z153" s="3">
         <v>2009502</v>
       </c>
-      <c r="AA153" s="63">
+      <c r="AA153" s="60">
         <v>2009502</v>
       </c>
     </row>
@@ -16933,7 +16933,7 @@
       <c r="Z154" s="3">
         <v>3942687</v>
       </c>
-      <c r="AA154" s="63">
+      <c r="AA154" s="60">
         <v>3942687</v>
       </c>
     </row>
@@ -17016,7 +17016,7 @@
       <c r="Z155" s="3">
         <v>1595530</v>
       </c>
-      <c r="AA155" s="63">
+      <c r="AA155" s="60">
         <v>1595530</v>
       </c>
     </row>
@@ -17099,7 +17099,7 @@
       <c r="Z156" s="3">
         <v>6895990</v>
       </c>
-      <c r="AA156" s="63">
+      <c r="AA156" s="60">
         <v>6895990</v>
       </c>
     </row>
@@ -17182,7 +17182,7 @@
       <c r="Z157" s="3">
         <v>1795923</v>
       </c>
-      <c r="AA157" s="63">
+      <c r="AA157" s="60">
         <v>1795923</v>
       </c>
     </row>
@@ -17265,7 +17265,7 @@
       <c r="Z158" s="3">
         <v>706215</v>
       </c>
-      <c r="AA158" s="63">
+      <c r="AA158" s="60">
         <v>706215</v>
       </c>
     </row>
@@ -17348,7 +17348,7 @@
       <c r="Z159" s="3">
         <v>56822</v>
       </c>
-      <c r="AA159" s="63">
+      <c r="AA159" s="60">
         <v>56822</v>
       </c>
     </row>
@@ -17431,7 +17431,7 @@
       <c r="Z160" s="3">
         <v>9342010</v>
       </c>
-      <c r="AA160" s="63">
+      <c r="AA160" s="60">
         <v>8736211</v>
       </c>
     </row>
@@ -17514,7 +17514,7 @@
       <c r="Z161" s="3">
         <v>3819520</v>
       </c>
-      <c r="AA161" s="63">
+      <c r="AA161" s="60">
         <v>3819520</v>
       </c>
     </row>
@@ -17597,7 +17597,7 @@
       <c r="Z162" s="3">
         <v>5513058</v>
       </c>
-      <c r="AA162" s="63">
+      <c r="AA162" s="60">
         <v>5513058</v>
       </c>
     </row>
@@ -17680,7 +17680,7 @@
       <c r="Z163" s="3">
         <v>1980910</v>
       </c>
-      <c r="AA163" s="63">
+      <c r="AA163" s="60">
         <v>1980910</v>
       </c>
     </row>
@@ -17763,7 +17763,7 @@
       <c r="Z164" s="3">
         <v>3168186</v>
       </c>
-      <c r="AA164" s="63">
+      <c r="AA164" s="60">
         <v>3168186</v>
       </c>
     </row>
@@ -17844,7 +17844,7 @@
         <v>82305</v>
       </c>
       <c r="Z165" s="5"/>
-      <c r="AA165" s="64"/>
+      <c r="AA165" s="61"/>
     </row>
     <row r="166" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A166" s="14">
@@ -17925,7 +17925,7 @@
       <c r="Z166" s="3">
         <v>385790</v>
       </c>
-      <c r="AA166" s="63">
+      <c r="AA166" s="60">
         <v>385790</v>
       </c>
     </row>
@@ -17992,7 +17992,7 @@
       <c r="X167" s="5"/>
       <c r="Y167" s="10"/>
       <c r="Z167" s="5"/>
-      <c r="AA167" s="64"/>
+      <c r="AA167" s="61"/>
     </row>
     <row r="168" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A168" s="14">
@@ -18073,7 +18073,7 @@
       <c r="Z168" s="3">
         <v>8393058</v>
       </c>
-      <c r="AA168" s="63">
+      <c r="AA168" s="60">
         <v>8308032</v>
       </c>
     </row>
@@ -18156,7 +18156,7 @@
       <c r="Z169" s="3">
         <v>2849630</v>
       </c>
-      <c r="AA169" s="63">
+      <c r="AA169" s="60">
         <v>2849630</v>
       </c>
     </row>
@@ -18239,7 +18239,7 @@
       <c r="Z170" s="3">
         <v>1024934</v>
       </c>
-      <c r="AA170" s="63">
+      <c r="AA170" s="60">
         <v>1024934</v>
       </c>
     </row>
@@ -18306,7 +18306,7 @@
       <c r="X171" s="5"/>
       <c r="Y171" s="10"/>
       <c r="Z171" s="5"/>
-      <c r="AA171" s="64"/>
+      <c r="AA171" s="61"/>
     </row>
     <row r="172" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A172" s="14">
@@ -18387,7 +18387,7 @@
       <c r="Z172" s="3">
         <v>5173290</v>
       </c>
-      <c r="AA172" s="63">
+      <c r="AA172" s="60">
         <v>5173290</v>
       </c>
     </row>
@@ -18470,7 +18470,7 @@
       <c r="Z173" s="3">
         <v>5625305</v>
       </c>
-      <c r="AA173" s="63">
+      <c r="AA173" s="60">
         <v>5625305</v>
       </c>
     </row>
@@ -18541,7 +18541,7 @@
       <c r="X174" s="5"/>
       <c r="Y174" s="10"/>
       <c r="Z174" s="5"/>
-      <c r="AA174" s="64"/>
+      <c r="AA174" s="61"/>
     </row>
     <row r="175" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A175" s="14">
@@ -18606,7 +18606,7 @@
       <c r="X175" s="5"/>
       <c r="Y175" s="10"/>
       <c r="Z175" s="5"/>
-      <c r="AA175" s="64"/>
+      <c r="AA175" s="61"/>
     </row>
     <row r="176" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A176" s="14">
@@ -18687,7 +18687,7 @@
       <c r="Z176" s="3">
         <v>3657325</v>
       </c>
-      <c r="AA176" s="63">
+      <c r="AA176" s="60">
         <v>3657325</v>
       </c>
     </row>
@@ -18770,7 +18770,7 @@
       <c r="Z177" s="3">
         <v>178933</v>
       </c>
-      <c r="AA177" s="63">
+      <c r="AA177" s="60">
         <v>178933</v>
       </c>
     </row>
@@ -18853,7 +18853,7 @@
       <c r="Z178" s="3">
         <v>1424815</v>
       </c>
-      <c r="AA178" s="63">
+      <c r="AA178" s="60">
         <v>1424815</v>
       </c>
     </row>
@@ -18936,7 +18936,7 @@
       <c r="Z179" s="3">
         <v>212034</v>
       </c>
-      <c r="AA179" s="63">
+      <c r="AA179" s="60">
         <v>212034</v>
       </c>
     </row>
@@ -19019,7 +19019,7 @@
       <c r="Z180" s="3">
         <v>1624007</v>
       </c>
-      <c r="AA180" s="63">
+      <c r="AA180" s="60">
         <v>1624007</v>
       </c>
     </row>
@@ -19102,7 +19102,7 @@
       <c r="Z181" s="3">
         <v>5418887</v>
       </c>
-      <c r="AA181" s="63">
+      <c r="AA181" s="60">
         <v>5418887</v>
       </c>
     </row>
@@ -19185,7 +19185,7 @@
       <c r="Z182" s="3">
         <v>215860</v>
       </c>
-      <c r="AA182" s="63">
+      <c r="AA182" s="60">
         <v>215860</v>
       </c>
     </row>
@@ -19268,7 +19268,7 @@
       <c r="Z183" s="3">
         <v>1581368</v>
       </c>
-      <c r="AA183" s="63">
+      <c r="AA183" s="60">
         <v>1581368</v>
       </c>
     </row>
@@ -19315,7 +19315,7 @@
       <c r="X184" s="5"/>
       <c r="Y184" s="10"/>
       <c r="Z184" s="5"/>
-      <c r="AA184" s="64"/>
+      <c r="AA184" s="61"/>
     </row>
     <row r="185" spans="1:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A185" s="14">
@@ -19396,7 +19396,7 @@
       <c r="Z185" s="3">
         <v>344901</v>
       </c>
-      <c r="AA185" s="63">
+      <c r="AA185" s="60">
         <v>344901</v>
       </c>
     </row>
@@ -19479,7 +19479,7 @@
       <c r="Z186" s="3">
         <v>143194</v>
       </c>
-      <c r="AA186" s="63">
+      <c r="AA186" s="60">
         <v>143194</v>
       </c>
     </row>
@@ -19562,7 +19562,7 @@
       <c r="Z187" s="3">
         <v>1149057</v>
       </c>
-      <c r="AA187" s="63">
+      <c r="AA187" s="60">
         <v>1149057</v>
       </c>
     </row>
@@ -19645,7 +19645,7 @@
       <c r="Z188" s="3">
         <v>369382</v>
       </c>
-      <c r="AA188" s="63">
+      <c r="AA188" s="60">
         <v>369382</v>
       </c>
     </row>
@@ -20222,10 +20222,10 @@
   <dimension ref="A1:AA187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="U106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="U5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AA4" sqref="AA4"/>
+      <selection pane="bottomRight" activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>